<commit_message>
copy updates; refactored titles, etc
</commit_message>
<xml_diff>
--- a/docs/CodeSystem-DeqmOperationOutcomeCodeSystem.xlsx
+++ b/docs/CodeSystem-DeqmOperationOutcomeCodeSystem.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://gitlab.mitre.org/awatson/water-closet-ig/CodeSystem/DeqmOperationOutcomeCodeSystem</t>
+    <t>https://github.com/clinical-meteor/r5-miscellaneous/CodeSystem/DeqmOperationOutcomeCodeSystem</t>
   </si>
   <si>
     <t>Version</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-22T23:10:47-05:00</t>
+    <t>2022-03-24T15:23:22-05:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>